<commit_message>
Se suben los issues y la nueva version 0.8
</commit_message>
<xml_diff>
--- a/Issues.xlsx
+++ b/Issues.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>Id</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>Se presenta la pantalla 5 para revisión</t>
+  </si>
+  <si>
+    <t>Pantalla 5: Pantalla de cabecera: La versión situarla arriba de la primer letra del nombre del usuario conectado.</t>
+  </si>
+  <si>
+    <t>Pantalla 5: Campo de Moneda. Entendemos que es una lista desplegable con las monedas configuradas en Netsuite.</t>
+  </si>
+  <si>
+    <t>0.8</t>
   </si>
 </sst>
 </file>
@@ -167,8 +176,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:F10" totalsRowShown="0" dataDxfId="6">
-  <autoFilter ref="A1:F10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:F12" totalsRowShown="0" dataDxfId="6">
+  <autoFilter ref="A1:F12">
     <filterColumn colId="4"/>
     <filterColumn colId="5"/>
   </autoFilter>
@@ -469,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -659,13 +668,49 @@
       <c r="C10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="5">
-        <v>0.7</v>
+      <c r="D10" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" ht="30">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" ht="45">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>